<commit_message>
Más pruebas de F3 en excel y test_access_manager_test.py (al cambiar el storageKey.json dejan de funcionar las pruebas) access_key.py guarda keys storageKey.json access_manager.py pequeña corrección
</commit_message>
<xml_diff>
--- a/docs/GE3_TestCasesTemplate_v1.0.xlsx
+++ b/docs/GE3_TestCasesTemplate_v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Universidad\2\2oCuatrimestre\Desarrollo de Software\EjerciciosGuiados\EG3\G81.T17.EG3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Universidad\2\2oCuatrimestre\Desarrollo de Software\EjerciciosGuiados\EG3\G81.T17.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D6E76-DA20-4AB2-BDE4-4CB264A49175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199F3701-C387-48BA-9E4B-A6BD8C2917F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="19524" windowHeight="10308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2021 F3" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>ID TEST</t>
   </si>
@@ -60,9 +60,6 @@
     <t>KEY</t>
   </si>
   <si>
-    <t>12341321413241324132412341324132</t>
-  </si>
-  <si>
     <t>1_2_3_4_6_7</t>
   </si>
   <si>
@@ -202,6 +199,21 @@
   </si>
   <si>
     <t>Fichero formato erroneo</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>1111111111111111111111111111111111111111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>821c9d9cf4ab2255fd53a8365042a12f49f183e82b811f8ae2dc3ebe941b3bb4</t>
   </si>
 </sst>
 </file>
@@ -258,13 +270,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -624,9 +637,10 @@
     <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" customWidth="1"/>
-    <col min="6" max="7" width="33.7265625" customWidth="1"/>
+    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7265625" customWidth="1"/>
     <col min="8" max="25" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -658,19 +672,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -679,16 +693,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -696,13 +714,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -713,16 +731,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -730,13 +752,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -747,16 +769,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -764,16 +790,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -781,16 +811,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -798,13 +832,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -815,13 +849,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -832,13 +866,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -849,13 +883,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -866,13 +900,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -883,13 +917,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -900,13 +934,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1"/>
@@ -917,13 +951,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2193,6 +2227,9 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E5" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>